<commit_message>
agrupamentos por estação, e agrupamento pela médias anual
</commit_message>
<xml_diff>
--- a/output/semivariogram-models.xlsx
+++ b/output/semivariogram-models.xlsx
@@ -527,26 +527,26 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Sph</t>
         </is>
       </c>
       <c r="C6">
-        <v>0.3891</v>
+        <v>0.6035</v>
       </c>
       <c r="D6">
-        <v>1.3781</v>
+        <v>1.3499</v>
       </c>
       <c r="E6">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="F6">
-        <v>0.2823452579638633</v>
+        <v>0.4470701533446922</v>
       </c>
       <c r="G6">
-        <v>8437.2984</v>
+        <v>840.9776000000001</v>
       </c>
       <c r="H6">
-        <v>0.7330696789932608</v>
+        <v>0.8457204115375917</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
análise final - tcc
</commit_message>
<xml_diff>
--- a/output/semivariogram-models.xlsx
+++ b/output/semivariogram-models.xlsx
@@ -407,26 +407,26 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Sph</t>
         </is>
       </c>
       <c r="C2">
-        <v>0.4708</v>
+        <v>0.5362</v>
       </c>
       <c r="D2">
-        <v>0.9671999999999999</v>
+        <v>0.9239000000000001</v>
       </c>
       <c r="E2">
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="F2">
-        <v>0.4867659222497933</v>
+        <v>0.5803658404589241</v>
       </c>
       <c r="G2">
-        <v>3218.2295</v>
+        <v>1743.5906</v>
       </c>
       <c r="H2">
-        <v>-0.2788779124871463</v>
+        <v>0.2931067733833046</v>
       </c>
     </row>
     <row r="3">

</xml_diff>